<commit_message>
Move electricity use from "H2 coal gasification + CCS" to CCS dataset Remove H2O use to CCS dataset Adjsut water balance.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-coal-gasification_CCS.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-coal-gasification_CCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0520BCEA-F3D9-D74A-9337-B4E5461DCA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BEDFEA-FB88-3B40-A2F5-1E7140311F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="72">
   <si>
     <t>Activity</t>
   </si>
@@ -206,15 +206,9 @@
     <t>From Li et al., 2022. For CCS.</t>
   </si>
   <si>
-    <t>market for tap water</t>
-  </si>
-  <si>
     <t>RoW</t>
   </si>
   <si>
-    <t>tap water</t>
-  </si>
-  <si>
     <t>From Li et al., 2022. For CCS. Originally called "cooling water", hence, may be from river or even the sea.</t>
   </si>
   <si>
@@ -236,18 +230,6 @@
     <t>Originally in megajoule. LHV: 120 MJ/kg. Originally: Wokaun A, Wilhelm E, Schenler W, Simons A, Bauer C, Bond S, et al. Transition to hydrogen - pathways toward clean transportation. New York: Cambridge University Press; 2011. Updated with: Jiaquan Li, Yi-Ming Wei, Lancui Liu, Xiaoyu Li, Rui Yan, The carbon footprint and cost of coal-based hydrogen production with and without carbon capture and storage technology in China, Journal of Cleaner Production, 2022, https://doi.org/10.1016/j.jclepro.2022.132514. Li et al., 2022, is based on an existing plant in China, and an existing CCS project in China. CO2 transport and storage is from Volkart et al., 2013.</t>
   </si>
   <si>
-    <t>Water, cooling, unspecified natural origin</t>
-  </si>
-  <si>
-    <t>natural resource::in water</t>
-  </si>
-  <si>
-    <t>From Li et al., 2022. For CCS. Originally called "desalted water", hence, desalination process is missing.</t>
-  </si>
-  <si>
-    <t>carbon dioxide, captured at hydrogen production plant, pre, pipeline 400km, storage 3000m</t>
-  </si>
-  <si>
     <t>Originally 8.99 kg coal/kg H2 in Li et al., 2022, we remove the supply chain losses to match the stoichiometric CO2 emissions of the process, since coal losses are already included in the upstream coal mining and supply datasets.</t>
   </si>
   <si>
@@ -267,6 +249,9 @@
   </si>
   <si>
     <t>methanol</t>
+  </si>
+  <si>
+    <t>carbon dioxide, captured at hydrogen production plant, pre, pipeline 200km, storage 1000m</t>
   </si>
 </sst>
 </file>
@@ -335,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -343,6 +328,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -643,7 +629,7 @@
         <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -651,7 +637,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -667,7 +653,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -691,7 +677,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -699,14 +685,14 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>47</v>
       </c>
     </row>
@@ -743,13 +729,13 @@
     </row>
     <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
@@ -761,7 +747,7 @@
         <v>19</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -772,7 +758,7 @@
         <v>10.5</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -789,82 +775,84 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B15">
-        <f>32/1000</f>
-        <v>3.2000000000000001E-2</v>
+        <f>0.008*1.2</f>
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="H15" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B16">
-        <v>10.24</v>
+        <f>0.057/1000</f>
+        <v>5.7000000000000003E-5</v>
       </c>
       <c r="C16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" t="s">
         <v>57</v>
       </c>
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" t="s">
-        <v>68</v>
-      </c>
       <c r="H16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="B17">
-        <f>0.008*1.2</f>
-        <v>9.5999999999999992E-3</v>
+        <v>6.9971999999999994E-10</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F17" t="s">
         <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="H17" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="B18">
-        <f>0.057/1000</f>
-        <v>5.7000000000000003E-5</v>
+        <v>0.16752</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
@@ -873,21 +861,21 @@
         <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="H18" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B19">
-        <v>6.9971999999999994E-10</v>
+        <v>3.9743999999999998E-9</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
@@ -896,21 +884,21 @@
         <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H19" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B20">
-        <v>0.16752</v>
+        <v>6.7709999999999999</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
         <v>13</v>
@@ -919,93 +907,95 @@
         <v>22</v>
       </c>
       <c r="G20" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="H20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B21">
-        <v>3.9743999999999998E-9</v>
+        <v>1.1397599999999999</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="F21" t="s">
         <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="H21" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B22">
-        <v>6.7709999999999999</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F22" t="s">
         <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="H22" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B23">
-        <v>1.1397599999999999</v>
+        <f>0.98/1000</f>
+        <v>9.7999999999999997E-4</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="F23" t="s">
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H23" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B24">
-        <v>4.3899999999999997</v>
+        <f>4.44/1000</f>
+        <v>4.4400000000000004E-3</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="F24" t="s">
         <v>22</v>
@@ -1014,42 +1004,41 @@
         <v>49</v>
       </c>
       <c r="H24" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B25">
-        <v>3.36</v>
+        <v>0.42432000000000003</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F25" t="s">
         <v>22</v>
       </c>
       <c r="G25" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B26">
-        <f>0.98/1000</f>
-        <v>9.7999999999999997E-4</v>
+        <v>-0.50531999999999999</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" t="s">
         <v>13</v>
@@ -1058,22 +1047,21 @@
         <v>22</v>
       </c>
       <c r="G26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H26" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="B27">
-        <f>4.44/1000</f>
-        <v>4.4400000000000004E-3</v>
+        <v>-0.22847999999999999</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" t="s">
         <v>13</v>
@@ -1082,212 +1070,152 @@
         <v>22</v>
       </c>
       <c r="G27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H27" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28">
-        <v>0.42432000000000003</v>
+        <v>52</v>
+      </c>
+      <c r="B28" s="3">
+        <f>(-B14/1000)</f>
+        <v>-1.0500000000000001E-2</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="F28" t="s">
         <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H28" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B29">
-        <v>-0.50531999999999999</v>
-      </c>
-      <c r="C29" t="s">
-        <v>57</v>
+        <v>6.9264000000000001E-3</v>
       </c>
       <c r="D29" t="s">
         <v>13</v>
       </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
       <c r="F29" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G29" t="s">
         <v>48</v>
       </c>
-      <c r="H29" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B30">
-        <v>-0.22847999999999999</v>
-      </c>
-      <c r="C30" t="s">
-        <v>57</v>
+        <v>2.48</v>
       </c>
       <c r="D30" t="s">
         <v>13</v>
       </c>
+      <c r="E30" t="s">
+        <v>14</v>
+      </c>
       <c r="F30" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>48</v>
-      </c>
-      <c r="H30" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="3">
-        <f>(-36.07/1000)+(-79/1000)</f>
-        <v>-0.11507000000000001</v>
-      </c>
-      <c r="C31" t="s">
-        <v>57</v>
+        <v>17</v>
+      </c>
+      <c r="B31">
+        <v>1.0375199999999999E-2</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
+        <v>13</v>
+      </c>
+      <c r="E31" t="s">
+        <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>55</v>
-      </c>
-      <c r="H31" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="B32">
-        <v>6.9264000000000001E-3</v>
+        <f>17.77-B30</f>
+        <v>15.29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
       </c>
-      <c r="E32" t="s">
-        <v>14</v>
-      </c>
       <c r="F32" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33">
-        <v>2.48</v>
-      </c>
-      <c r="D33" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" t="s">
-        <v>49</v>
+        <v>62</v>
+      </c>
+      <c r="H32" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34">
-        <v>1.0375199999999999E-2</v>
-      </c>
-      <c r="D34" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35">
-        <f>17.77-B33</f>
-        <v>15.29</v>
-      </c>
-      <c r="C35" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" t="s">
-        <v>22</v>
-      </c>
-      <c r="G35" t="s">
-        <v>64</v>
-      </c>
-      <c r="H35" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="4"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-    </row>
-    <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="1"/>
-      <c r="B56" s="4"/>
-    </row>
-    <row r="64" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="4"/>
+    </row>
+    <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B65" s="5"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B66" s="5"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B67" s="5"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B68" s="5"/>
@@ -1295,22 +1223,13 @@
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B69" s="5"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="2"/>
       <c r="B70" s="5"/>
+      <c r="G70" s="2"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B71" s="5"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B72" s="5"/>
-    </row>
-    <row r="73" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="2"/>
-      <c r="B73" s="5"/>
-      <c r="G73" s="2"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B74" s="3"/>
+      <c r="B71" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Fix water and electricity requirements for CCS on H2 production. Set gas input to H2 from SMR to national market.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-coal-gasification_CCS.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-coal-gasification_CCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BEDFEA-FB88-3B40-A2F5-1E7140311F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B3E7A5-D81B-4F49-A88C-3853E7F38047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6440" yWindow="1400" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="79">
   <si>
     <t>Activity</t>
   </si>
@@ -209,9 +209,6 @@
     <t>RoW</t>
   </si>
   <si>
-    <t>From Li et al., 2022. For CCS. Originally called "cooling water", hence, may be from river or even the sea.</t>
-  </si>
-  <si>
     <t>market for ammonia, anhydrous, liquid</t>
   </si>
   <si>
@@ -252,6 +249,30 @@
   </si>
   <si>
     <t>carbon dioxide, captured at hydrogen production plant, pre, pipeline 200km, storage 1000m</t>
+  </si>
+  <si>
+    <t>From Li et al., 2022. Electricity for CCS.</t>
+  </si>
+  <si>
+    <t>Water, cooling, unspecified natural origin</t>
+  </si>
+  <si>
+    <t>natural resource::in water</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve">From Li et al., 2022. For CCS. </t>
+  </si>
+  <si>
+    <t>From Li et al., 2022. For CCS. Listed as "desalted water".</t>
+  </si>
+  <si>
+    <t>From Li et al., 2022. For CCS. Amount of freshwater consumed per kg CO2 captured for cooling.</t>
+  </si>
+  <si>
+    <t>From Li et al., 2022. For CCS. Treatment of freshwater. Amount of freshwater treated and released back to water per kg CO2 captured. Assumes the equivalent of 600 gallons of water evaporated/t CO2 captured, hence not treated.</t>
   </si>
 </sst>
 </file>
@@ -320,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -328,7 +349,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -621,6 +641,7 @@
     <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
     <col min="9" max="9" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -629,7 +650,7 @@
         <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -637,7 +658,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -653,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -685,14 +706,14 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" t="s">
         <v>47</v>
       </c>
     </row>
@@ -729,7 +750,7 @@
     </row>
     <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -747,78 +768,7 @@
         <v>19</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14">
-        <v>10.5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15">
-        <f>0.008*1.2</f>
-        <v>9.5999999999999992E-3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16">
-        <f>0.057/1000</f>
-        <v>5.7000000000000003E-5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -907,7 +857,7 @@
         <v>22</v>
       </c>
       <c r="G20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H20" t="s">
         <v>31</v>
@@ -944,7 +894,7 @@
         <v>4.3899999999999997</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
         <v>36</v>
@@ -985,7 +935,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24">
         <f>4.44/1000</f>
@@ -1004,7 +954,7 @@
         <v>49</v>
       </c>
       <c r="H24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1081,8 +1031,8 @@
         <v>52</v>
       </c>
       <c r="B28" s="3">
-        <f>(-B14/1000)</f>
-        <v>-1.0500000000000001E-2</v>
+        <f>(-B35/1000)</f>
+        <v>-1.0240000000000001E-2</v>
       </c>
       <c r="C28" t="s">
         <v>56</v>
@@ -1162,7 +1112,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32">
         <f>17.77-B30</f>
@@ -1178,35 +1128,176 @@
         <v>22</v>
       </c>
       <c r="G32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>3.36</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34">
+        <f>32/1000</f>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" t="s">
+        <v>77</v>
+      </c>
+      <c r="I34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <v>10.24</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" t="s">
+        <v>76</v>
+      </c>
+      <c r="H35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="5">
+        <f>(((B34*1000)+B35-(600*3.78541/1000))/1000)*-1</f>
+        <v>-3.9968754000000002E-2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37">
+        <f>0.008*1.2</f>
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" t="s">
+        <v>75</v>
+      </c>
+      <c r="H37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38">
+        <f>0.057/1000</f>
+        <v>5.7000000000000003E-5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" t="s">
+        <v>55</v>
+      </c>
+      <c r="H38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
-      <c r="B53" s="4"/>
-    </row>
-    <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="1"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="4"/>
+    </row>
+    <row r="60" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B65" s="5"/>
@@ -1220,16 +1311,13 @@
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B68" s="5"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="2"/>
       <c r="B69" s="5"/>
-    </row>
-    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="2"/>
-      <c r="B70" s="5"/>
-      <c r="G70" s="2"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B71" s="3"/>
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B70" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>